<commit_message>
fixed 113 signs symptoms resident files
</commit_message>
<xml_diff>
--- a/113 symptoms signs abnormal/RES 113 symptoms signs abnormal Findings ethnicity 2020Jul19.XLSX
+++ b/113 symptoms signs abnormal/RES 113 symptoms signs abnormal Findings ethnicity 2020Jul19.XLSX
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bague\Documents\GitHub\FLHealthCHARTS\113 symptoms signs abnormal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bague\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F234F90C-8874-45D1-9FD1-0550EABA8CDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53B8491B-960B-4F0C-A982-7A7DEF3C0DFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Recovered_Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
-    <t>Recorded Deaths by Year by Ethnicity by Residence County</t>
+    <t>Resident Death Counts by Year by Ethnicity by Residence County</t>
   </si>
   <si>
     <t>113 Causes of Death=Symptoms, Signs &amp; Abnormal Findings</t>
   </si>
   <si>
-    <t>Recorded Deaths</t>
+    <t>Resident Deaths</t>
   </si>
   <si>
     <t>2020 (Provisional)</t>
@@ -1214,20 +1214,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1330,40 +1330,40 @@
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F6" s="2">
         <v>4</v>
       </c>
       <c r="G6" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J6" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K6" s="2">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L6" s="2">
         <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="N6" s="2">
-        <v>176</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1418,40 +1418,40 @@
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
       </c>
       <c r="I8" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J8" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K8" s="2">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="L8" s="2">
         <v>1</v>
       </c>
       <c r="M8" s="2">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="N8" s="2">
-        <v>88</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1486,16 +1486,16 @@
         <v>0</v>
       </c>
       <c r="K9" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L9" s="2">
         <v>0</v>
       </c>
       <c r="M9" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N9" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1503,43 +1503,43 @@
         <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F10" s="2">
         <v>4</v>
       </c>
       <c r="G10" s="2">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H10" s="2">
         <v>4</v>
       </c>
       <c r="I10" s="2">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="J10" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K10" s="2">
-        <v>148</v>
+        <v>194</v>
       </c>
       <c r="L10" s="2">
         <v>7</v>
       </c>
       <c r="M10" s="2">
-        <v>163</v>
+        <v>211</v>
       </c>
       <c r="N10" s="2">
-        <v>290</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1550,40 +1550,40 @@
         <v>10</v>
       </c>
       <c r="C11" s="2">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="D11" s="2">
         <v>5</v>
       </c>
       <c r="E11" s="2">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="F11" s="2">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G11" s="2">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="H11" s="2">
         <v>3</v>
       </c>
       <c r="I11" s="2">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="J11" s="2">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K11" s="2">
-        <v>170</v>
+        <v>268</v>
       </c>
       <c r="L11" s="2">
         <v>16</v>
       </c>
       <c r="M11" s="2">
-        <v>213</v>
+        <v>317</v>
       </c>
       <c r="N11" s="2">
-        <v>376</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1618,16 +1618,16 @@
         <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
       </c>
       <c r="M12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1638,40 +1638,40 @@
         <v>1</v>
       </c>
       <c r="C13" s="2">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
       </c>
       <c r="E13" s="2">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F13" s="2">
         <v>2</v>
       </c>
       <c r="G13" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J13" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K13" s="2">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="L13" s="2">
         <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="N13" s="2">
-        <v>103</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1682,13 +1682,13 @@
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -1703,19 +1703,19 @@
         <v>23</v>
       </c>
       <c r="J14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="L14" s="2">
         <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="N14" s="2">
-        <v>74</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1726,13 +1726,13 @@
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2">
         <v>4</v>
       </c>
       <c r="E15" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -1741,25 +1741,25 @@
         <v>19</v>
       </c>
       <c r="H15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L15" s="2">
         <v>2</v>
       </c>
       <c r="M15" s="2">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="N15" s="2">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1770,40 +1770,40 @@
         <v>3</v>
       </c>
       <c r="C16" s="2">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F16" s="2">
         <v>4</v>
       </c>
       <c r="G16" s="2">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H16" s="2">
         <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J16" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K16" s="2">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
       </c>
       <c r="M16" s="2">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="N16" s="2">
-        <v>111</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1838,16 +1838,16 @@
         <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L17" s="2">
         <v>1</v>
       </c>
       <c r="M17" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N17" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1855,43 +1855,43 @@
         <v>20</v>
       </c>
       <c r="B18" s="2">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2">
         <v>4</v>
       </c>
       <c r="E18" s="2">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="F18" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G18" s="2">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="2">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="J18" s="2">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="K18" s="2">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="L18" s="2">
         <v>7</v>
       </c>
       <c r="M18" s="2">
-        <v>182</v>
+        <v>245</v>
       </c>
       <c r="N18" s="2">
-        <v>376</v>
+        <v>464</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1902,13 +1902,13 @@
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
@@ -1935,7 +1935,7 @@
         <v>6</v>
       </c>
       <c r="N19" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1970,16 +1970,16 @@
         <v>0</v>
       </c>
       <c r="K20" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
       </c>
       <c r="M20" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N20" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -1990,40 +1990,40 @@
         <v>4</v>
       </c>
       <c r="C21" s="2">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D21" s="2">
         <v>5</v>
       </c>
       <c r="E21" s="2">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="2">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H21" s="2">
         <v>4</v>
       </c>
       <c r="I21" s="2">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J21" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K21" s="2">
-        <v>98</v>
+        <v>161</v>
       </c>
       <c r="L21" s="2">
         <v>11</v>
       </c>
       <c r="M21" s="2">
-        <v>114</v>
+        <v>178</v>
       </c>
       <c r="N21" s="2">
-        <v>267</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2034,40 +2034,40 @@
         <v>1</v>
       </c>
       <c r="C22" s="2">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
       </c>
       <c r="E22" s="2">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H22" s="2">
         <v>1</v>
       </c>
       <c r="I22" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K22" s="2">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="L22" s="2">
         <v>0</v>
       </c>
       <c r="M22" s="2">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="N22" s="2">
-        <v>114</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2078,40 +2078,40 @@
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
       </c>
       <c r="G23" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
       </c>
       <c r="I23" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J23" s="2">
         <v>0</v>
       </c>
       <c r="K23" s="2">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="L23" s="2">
         <v>0</v>
       </c>
       <c r="M23" s="2">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="N23" s="2">
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2122,25 +2122,25 @@
         <v>0</v>
       </c>
       <c r="C24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>
       </c>
       <c r="E24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
       </c>
       <c r="G24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
       <c r="I24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J24" s="2">
         <v>0</v>
@@ -2155,7 +2155,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2190,16 +2190,16 @@
         <v>1</v>
       </c>
       <c r="K25" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L25" s="2">
         <v>0</v>
       </c>
       <c r="M25" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N25" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2298,40 +2298,40 @@
         <v>0</v>
       </c>
       <c r="C28" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
       </c>
       <c r="E28" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
       </c>
       <c r="G28" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J28" s="2">
         <v>0</v>
       </c>
       <c r="K28" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L28" s="2">
         <v>0</v>
       </c>
       <c r="M28" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N28" s="2">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2366,16 +2366,16 @@
         <v>1</v>
       </c>
       <c r="K29" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L29" s="2">
         <v>0</v>
       </c>
       <c r="M29" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N29" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2386,13 +2386,13 @@
         <v>0</v>
       </c>
       <c r="C30" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
       </c>
       <c r="E30" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30" s="2">
         <v>0</v>
@@ -2410,16 +2410,16 @@
         <v>1</v>
       </c>
       <c r="K30" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L30" s="2">
         <v>0</v>
       </c>
       <c r="M30" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N30" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2430,13 +2430,13 @@
         <v>0</v>
       </c>
       <c r="C31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
       </c>
       <c r="E31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="2">
         <v>0</v>
@@ -2451,19 +2451,19 @@
         <v>0</v>
       </c>
       <c r="J31" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K31" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L31" s="2">
         <v>0</v>
       </c>
       <c r="M31" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N31" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2474,40 +2474,40 @@
         <v>5</v>
       </c>
       <c r="C32" s="2">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D32" s="2">
         <v>3</v>
       </c>
       <c r="E32" s="2">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F32" s="2">
         <v>6</v>
       </c>
       <c r="G32" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H32" s="2">
         <v>1</v>
       </c>
       <c r="I32" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J32" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K32" s="2">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="L32" s="2">
         <v>0</v>
       </c>
       <c r="M32" s="2">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="N32" s="2">
-        <v>333</v>
+        <v>360</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2530,28 +2530,28 @@
         <v>1</v>
       </c>
       <c r="G33" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
       </c>
       <c r="I33" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J33" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K33" s="2">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="L33" s="2">
         <v>1</v>
       </c>
       <c r="M33" s="2">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="N33" s="2">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2559,43 +2559,43 @@
         <v>36</v>
       </c>
       <c r="B34" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C34" s="2">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D34" s="2">
         <v>0</v>
       </c>
       <c r="E34" s="2">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="F34" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G34" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
       </c>
       <c r="I34" s="2">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="J34" s="2">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="K34" s="2">
-        <v>264</v>
+        <v>319</v>
       </c>
       <c r="L34" s="2">
         <v>0</v>
       </c>
       <c r="M34" s="2">
-        <v>328</v>
+        <v>393</v>
       </c>
       <c r="N34" s="2">
-        <v>680</v>
+        <v>760</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2606,40 +2606,40 @@
         <v>0</v>
       </c>
       <c r="C35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
       </c>
       <c r="E35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="2">
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
       </c>
       <c r="I35" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J35" s="2">
         <v>0</v>
       </c>
       <c r="K35" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L35" s="2">
         <v>0</v>
       </c>
       <c r="M35" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N35" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2647,43 +2647,43 @@
         <v>38</v>
       </c>
       <c r="B36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="2">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D36" s="2">
         <v>1</v>
       </c>
       <c r="E36" s="2">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
       </c>
       <c r="G36" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
       </c>
       <c r="I36" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J36" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K36" s="2">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="L36" s="2">
         <v>0</v>
       </c>
       <c r="M36" s="2">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="N36" s="2">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2694,40 +2694,40 @@
         <v>1</v>
       </c>
       <c r="C37" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
       </c>
       <c r="E37" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F37" s="2">
         <v>0</v>
       </c>
       <c r="G37" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H37" s="2">
         <v>0</v>
       </c>
       <c r="I37" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J37" s="2">
         <v>2</v>
       </c>
       <c r="K37" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="L37" s="2">
         <v>0</v>
       </c>
       <c r="M37" s="2">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="N37" s="2">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2738,40 +2738,40 @@
         <v>0</v>
       </c>
       <c r="C38" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
       </c>
       <c r="E38" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F38" s="2">
         <v>0</v>
       </c>
       <c r="G38" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H38" s="2">
         <v>0</v>
       </c>
       <c r="I38" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J38" s="2">
         <v>0</v>
       </c>
       <c r="K38" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L38" s="2">
         <v>0</v>
       </c>
       <c r="M38" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N38" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2823,43 +2823,43 @@
         <v>42</v>
       </c>
       <c r="B40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D40" s="2">
         <v>0</v>
       </c>
       <c r="E40" s="2">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F40" s="2">
         <v>2</v>
       </c>
       <c r="G40" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H40" s="2">
         <v>0</v>
       </c>
       <c r="I40" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J40" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K40" s="2">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="L40" s="2">
         <v>1</v>
       </c>
       <c r="M40" s="2">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="N40" s="2">
-        <v>59</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2867,43 +2867,43 @@
         <v>43</v>
       </c>
       <c r="B41" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C41" s="2">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D41" s="2">
         <v>0</v>
       </c>
       <c r="E41" s="2">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="F41" s="2">
         <v>1</v>
       </c>
       <c r="G41" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H41" s="2">
         <v>0</v>
       </c>
       <c r="I41" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J41" s="2">
         <v>7</v>
       </c>
       <c r="K41" s="2">
-        <v>71</v>
+        <v>182</v>
       </c>
       <c r="L41" s="2">
         <v>1</v>
       </c>
       <c r="M41" s="2">
-        <v>79</v>
+        <v>190</v>
       </c>
       <c r="N41" s="2">
-        <v>167</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2914,13 +2914,13 @@
         <v>1</v>
       </c>
       <c r="C42" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D42" s="2">
         <v>0</v>
       </c>
       <c r="E42" s="2">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F42" s="2">
         <v>1</v>
@@ -2938,16 +2938,16 @@
         <v>0</v>
       </c>
       <c r="K42" s="2">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="L42" s="2">
         <v>0</v>
       </c>
       <c r="M42" s="2">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="N42" s="2">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2970,13 +2970,13 @@
         <v>1</v>
       </c>
       <c r="G43" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
       </c>
       <c r="I43" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J43" s="2">
         <v>1</v>
@@ -2991,7 +2991,7 @@
         <v>19</v>
       </c>
       <c r="N43" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3046,13 +3046,13 @@
         <v>0</v>
       </c>
       <c r="C45" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" s="2">
         <v>0</v>
       </c>
       <c r="E45" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F45" s="2">
         <v>0</v>
@@ -3070,16 +3070,16 @@
         <v>0</v>
       </c>
       <c r="K45" s="2">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L45" s="2">
         <v>0</v>
       </c>
       <c r="M45" s="2">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="N45" s="2">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3090,40 +3090,40 @@
         <v>5</v>
       </c>
       <c r="C46" s="2">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D46" s="2">
         <v>0</v>
       </c>
       <c r="E46" s="2">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="F46" s="2">
         <v>4</v>
       </c>
       <c r="G46" s="2">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
       </c>
       <c r="I46" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J46" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K46" s="2">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="L46" s="2">
         <v>0</v>
       </c>
       <c r="M46" s="2">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="N46" s="2">
-        <v>201</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3134,40 +3134,40 @@
         <v>3</v>
       </c>
       <c r="C47" s="2">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D47" s="2">
         <v>0</v>
       </c>
       <c r="E47" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F47" s="2">
         <v>6</v>
       </c>
       <c r="G47" s="2">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H47" s="2">
         <v>2</v>
       </c>
       <c r="I47" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J47" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K47" s="2">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="L47" s="2">
         <v>0</v>
       </c>
       <c r="M47" s="2">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="N47" s="2">
-        <v>224</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3178,40 +3178,40 @@
         <v>0</v>
       </c>
       <c r="C48" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D48" s="2">
         <v>0</v>
       </c>
       <c r="E48" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F48" s="2">
         <v>0</v>
       </c>
       <c r="G48" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H48" s="2">
         <v>0</v>
       </c>
       <c r="I48" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" s="2">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="L48" s="2">
         <v>1</v>
       </c>
       <c r="M48" s="2">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="N48" s="2">
-        <v>28</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3222,13 +3222,13 @@
         <v>0</v>
       </c>
       <c r="C49" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D49" s="2">
         <v>0</v>
       </c>
       <c r="E49" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F49" s="2">
         <v>2</v>
@@ -3246,16 +3246,16 @@
         <v>3</v>
       </c>
       <c r="K49" s="2">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="L49" s="2">
         <v>0</v>
       </c>
       <c r="M49" s="2">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="N49" s="2">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3266,40 +3266,40 @@
         <v>0</v>
       </c>
       <c r="C50" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D50" s="2">
         <v>0</v>
       </c>
       <c r="E50" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F50" s="2">
         <v>0</v>
       </c>
       <c r="G50" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H50" s="2">
         <v>1</v>
       </c>
       <c r="I50" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J50" s="2">
         <v>2</v>
       </c>
       <c r="K50" s="2">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="L50" s="2">
         <v>1</v>
       </c>
       <c r="M50" s="2">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="N50" s="2">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3310,40 +3310,40 @@
         <v>2</v>
       </c>
       <c r="C51" s="2">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D51" s="2">
         <v>1</v>
       </c>
       <c r="E51" s="2">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F51" s="2">
         <v>0</v>
       </c>
       <c r="G51" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H51" s="2">
         <v>0</v>
       </c>
       <c r="I51" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J51" s="2">
         <v>2</v>
       </c>
       <c r="K51" s="2">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="L51" s="2">
         <v>0</v>
       </c>
       <c r="M51" s="2">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="N51" s="2">
-        <v>78</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3354,13 +3354,13 @@
         <v>1</v>
       </c>
       <c r="C52" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D52" s="2">
         <v>0</v>
       </c>
       <c r="E52" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F52" s="2">
         <v>0</v>
@@ -3375,19 +3375,19 @@
         <v>18</v>
       </c>
       <c r="J52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L52" s="2">
         <v>1</v>
       </c>
       <c r="M52" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N52" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3395,43 +3395,43 @@
         <v>55</v>
       </c>
       <c r="B53" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C53" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D53" s="2">
         <v>2</v>
       </c>
       <c r="E53" s="2">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F53" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G53" s="2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H53" s="2">
         <v>0</v>
       </c>
       <c r="I53" s="2">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="J53" s="2">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K53" s="2">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="L53" s="2">
         <v>0</v>
       </c>
       <c r="M53" s="2">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="N53" s="2">
-        <v>205</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3439,43 +3439,43 @@
         <v>56</v>
       </c>
       <c r="B54" s="2">
+        <v>8</v>
+      </c>
+      <c r="C54" s="2">
+        <v>19</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2">
+        <v>27</v>
+      </c>
+      <c r="F54" s="2">
         <v>6</v>
       </c>
-      <c r="C54" s="2">
-        <v>15</v>
-      </c>
-      <c r="D54" s="2">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2">
-        <v>21</v>
-      </c>
-      <c r="F54" s="2">
-        <v>5</v>
-      </c>
       <c r="G54" s="2">
+        <v>13</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="2">
+        <v>19</v>
+      </c>
+      <c r="J54" s="2">
         <v>12</v>
       </c>
-      <c r="H54" s="2">
-        <v>0</v>
-      </c>
-      <c r="I54" s="2">
-        <v>17</v>
-      </c>
-      <c r="J54" s="2">
-        <v>6</v>
-      </c>
       <c r="K54" s="2">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="L54" s="2">
         <v>0</v>
       </c>
       <c r="M54" s="2">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="N54" s="2">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3486,40 +3486,40 @@
         <v>7</v>
       </c>
       <c r="C55" s="2">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="D55" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E55" s="2">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="F55" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G55" s="2">
+        <v>91</v>
+      </c>
+      <c r="H55" s="2">
+        <v>1</v>
+      </c>
+      <c r="I55" s="2">
+        <v>100</v>
+      </c>
+      <c r="J55" s="2">
         <v>68</v>
       </c>
-      <c r="H55" s="2">
-        <v>1</v>
-      </c>
-      <c r="I55" s="2">
-        <v>76</v>
-      </c>
-      <c r="J55" s="2">
-        <v>61</v>
-      </c>
       <c r="K55" s="2">
-        <v>312</v>
+        <v>462</v>
       </c>
       <c r="L55" s="2">
         <v>4</v>
       </c>
       <c r="M55" s="2">
-        <v>377</v>
+        <v>534</v>
       </c>
       <c r="N55" s="2">
-        <v>531</v>
+        <v>769</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3530,40 +3530,40 @@
         <v>12</v>
       </c>
       <c r="C56" s="2">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="D56" s="2">
         <v>2</v>
       </c>
       <c r="E56" s="2">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="F56" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G56" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="H56" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I56" s="2">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="J56" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K56" s="2">
-        <v>167</v>
+        <v>203</v>
       </c>
       <c r="L56" s="2">
         <v>2</v>
       </c>
       <c r="M56" s="2">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="N56" s="2">
-        <v>679</v>
+        <v>737</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3574,40 +3574,40 @@
         <v>25</v>
       </c>
       <c r="C57" s="5">
-        <v>1048</v>
+        <v>1062</v>
       </c>
       <c r="D57" s="2">
         <v>3</v>
       </c>
       <c r="E57" s="5">
-        <v>1076</v>
+        <v>1090</v>
       </c>
       <c r="F57" s="2">
         <v>36</v>
       </c>
-      <c r="G57" s="2">
-        <v>995</v>
+      <c r="G57" s="5">
+        <v>1002</v>
       </c>
       <c r="H57" s="2">
         <v>7</v>
       </c>
       <c r="I57" s="5">
-        <v>1038</v>
+        <v>1045</v>
       </c>
       <c r="J57" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K57" s="2">
-        <v>631</v>
+        <v>697</v>
       </c>
       <c r="L57" s="2">
         <v>3</v>
       </c>
       <c r="M57" s="2">
-        <v>658</v>
+        <v>725</v>
       </c>
       <c r="N57" s="5">
-        <v>2772</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3618,40 +3618,40 @@
         <v>4</v>
       </c>
       <c r="C58" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D58" s="2">
         <v>0</v>
       </c>
       <c r="E58" s="2">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F58" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G58" s="2">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H58" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" s="2">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="J58" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K58" s="2">
-        <v>159</v>
+        <v>201</v>
       </c>
       <c r="L58" s="2">
         <v>1</v>
       </c>
       <c r="M58" s="2">
-        <v>185</v>
+        <v>228</v>
       </c>
       <c r="N58" s="2">
-        <v>284</v>
+        <v>339</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3662,13 +3662,13 @@
         <v>0</v>
       </c>
       <c r="C59" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D59" s="2">
         <v>0</v>
       </c>
       <c r="E59" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F59" s="2">
         <v>0</v>
@@ -3686,16 +3686,16 @@
         <v>0</v>
       </c>
       <c r="K59" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L59" s="2">
         <v>0</v>
       </c>
       <c r="M59" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="N59" s="2">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3706,40 +3706,40 @@
         <v>1</v>
       </c>
       <c r="C60" s="2">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D60" s="2">
         <v>0</v>
       </c>
       <c r="E60" s="2">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F60" s="2">
         <v>0</v>
       </c>
       <c r="G60" s="2">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H60" s="2">
         <v>0</v>
       </c>
       <c r="I60" s="2">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J60" s="2">
         <v>0</v>
       </c>
       <c r="K60" s="2">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="L60" s="2">
         <v>0</v>
       </c>
       <c r="M60" s="2">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="N60" s="2">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3750,40 +3750,40 @@
         <v>4</v>
       </c>
       <c r="C61" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
       </c>
       <c r="E61" s="2">
+        <v>18</v>
+      </c>
+      <c r="F61" s="2">
+        <v>3</v>
+      </c>
+      <c r="G61" s="2">
+        <v>13</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0</v>
+      </c>
+      <c r="I61" s="2">
         <v>16</v>
       </c>
-      <c r="F61" s="2">
-        <v>2</v>
-      </c>
-      <c r="G61" s="2">
-        <v>10</v>
-      </c>
-      <c r="H61" s="2">
-        <v>0</v>
-      </c>
-      <c r="I61" s="2">
-        <v>12</v>
-      </c>
       <c r="J61" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K61" s="2">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="L61" s="2">
         <v>2</v>
       </c>
       <c r="M61" s="2">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="N61" s="2">
-        <v>64</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3794,13 +3794,13 @@
         <v>0</v>
       </c>
       <c r="C62" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D62" s="2">
         <v>0</v>
       </c>
       <c r="E62" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F62" s="2">
         <v>1</v>
@@ -3818,16 +3818,16 @@
         <v>1</v>
       </c>
       <c r="K62" s="2">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="L62" s="2">
         <v>0</v>
       </c>
       <c r="M62" s="2">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="N62" s="2">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3838,40 +3838,40 @@
         <v>4</v>
       </c>
       <c r="C63" s="2">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="D63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" s="2">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="F63" s="2">
         <v>3</v>
       </c>
       <c r="G63" s="2">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H63" s="2">
         <v>0</v>
       </c>
       <c r="I63" s="2">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="J63" s="2">
         <v>2</v>
       </c>
       <c r="K63" s="2">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="L63" s="2">
         <v>0</v>
       </c>
       <c r="M63" s="2">
-        <v>146</v>
+        <v>217</v>
       </c>
       <c r="N63" s="2">
-        <v>370</v>
+        <v>466</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3882,40 +3882,40 @@
         <v>2</v>
       </c>
       <c r="C64" s="2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D64" s="2">
         <v>0</v>
       </c>
       <c r="E64" s="2">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F64" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G64" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H64" s="2">
         <v>1</v>
       </c>
       <c r="I64" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J64" s="2">
         <v>1</v>
       </c>
       <c r="K64" s="2">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="L64" s="2">
         <v>0</v>
       </c>
       <c r="M64" s="2">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="N64" s="2">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3926,40 +3926,40 @@
         <v>0</v>
       </c>
       <c r="C65" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D65" s="2">
         <v>0</v>
       </c>
       <c r="E65" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F65" s="2">
         <v>0</v>
       </c>
       <c r="G65" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H65" s="2">
         <v>0</v>
       </c>
       <c r="I65" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J65" s="2">
         <v>1</v>
       </c>
       <c r="K65" s="2">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="L65" s="2">
         <v>0</v>
       </c>
       <c r="M65" s="2">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="N65" s="2">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -3967,7 +3967,7 @@
         <v>68</v>
       </c>
       <c r="B66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66" s="2">
         <v>11</v>
@@ -3976,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F66" s="2">
         <v>0</v>
@@ -3994,16 +3994,16 @@
         <v>0</v>
       </c>
       <c r="K66" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L66" s="2">
         <v>0</v>
       </c>
       <c r="M66" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N66" s="2">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -4082,16 +4082,16 @@
         <v>0</v>
       </c>
       <c r="K68" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L68" s="2">
         <v>0</v>
       </c>
       <c r="M68" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N68" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -4102,40 +4102,40 @@
         <v>2</v>
       </c>
       <c r="C69" s="2">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D69" s="2">
         <v>0</v>
       </c>
       <c r="E69" s="2">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F69" s="2">
         <v>0</v>
       </c>
       <c r="G69" s="2">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="H69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="J69" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K69" s="2">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="L69" s="2">
         <v>1</v>
       </c>
       <c r="M69" s="2">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="N69" s="2">
-        <v>123</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -4170,16 +4170,16 @@
         <v>0</v>
       </c>
       <c r="K70" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L70" s="2">
         <v>0</v>
       </c>
       <c r="M70" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N70" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -4190,40 +4190,40 @@
         <v>0</v>
       </c>
       <c r="C71" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
       </c>
       <c r="E71" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F71" s="2">
         <v>0</v>
       </c>
       <c r="G71" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H71" s="2">
         <v>0</v>
       </c>
       <c r="I71" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J71" s="2">
         <v>1</v>
       </c>
       <c r="K71" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L71" s="2">
         <v>0</v>
       </c>
       <c r="M71" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="N71" s="2">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -4258,16 +4258,16 @@
         <v>0</v>
       </c>
       <c r="K72" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L72" s="2">
         <v>0</v>
       </c>
       <c r="M72" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N72" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -4275,43 +4275,43 @@
         <v>7</v>
       </c>
       <c r="B73" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C73" s="2">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="D73" s="2">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="E73" s="2">
-        <v>141</v>
+        <v>5</v>
       </c>
       <c r="F73" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G73" s="2">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="H73" s="2">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="I73" s="2">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="J73" s="2">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K73" s="2">
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="L73" s="2">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="M73" s="2">
-        <v>249</v>
+        <v>1</v>
       </c>
       <c r="N73" s="2">
-        <v>517</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -4319,43 +4319,43 @@
         <v>4</v>
       </c>
       <c r="B74" s="3">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C74" s="6">
-        <v>2740</v>
+        <v>3034</v>
       </c>
       <c r="D74" s="3">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E74" s="6">
-        <v>3008</v>
+        <v>3279</v>
       </c>
       <c r="F74" s="3">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="G74" s="6">
-        <v>2992</v>
+        <v>3064</v>
       </c>
       <c r="H74" s="3">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="I74" s="6">
-        <v>3301</v>
+        <v>3345</v>
       </c>
       <c r="J74" s="3">
-        <v>431</v>
+        <v>499</v>
       </c>
       <c r="K74" s="6">
-        <v>3474</v>
+        <v>4852</v>
       </c>
       <c r="L74" s="3">
-        <v>127</v>
+        <v>66</v>
       </c>
       <c r="M74" s="6">
-        <v>4032</v>
+        <v>5417</v>
       </c>
       <c r="N74" s="6">
-        <v>10341</v>
+        <v>12041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>